<commit_message>
Created kmeans grouper and labeler.
</commit_message>
<xml_diff>
--- a/examples/tested.xlsx
+++ b/examples/tested.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -551,7 +551,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>POSITIVE</t>
+          <t>NEUTRAL</t>
         </is>
       </c>
     </row>
@@ -571,7 +571,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>nas</t>
+          <t>elonmusk</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -596,12 +596,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>nas</t>
+          <t>elonmusk</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>POSITIVE</t>
+          <t>NEUTRAL</t>
         </is>
       </c>
     </row>
@@ -621,10 +621,85 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>elonmusk</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>NEGATIVE</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>twitter is amazing</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>4,5,6</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
           <t>nas</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>POSITIVE</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>I hate twitter.</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>4,5,6</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nas</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>NEGATIVE</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>I dunno</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>4,5,6</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nas</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>NEGATIVE</t>
         </is>

</xml_diff>